<commit_message>
Added API for BookCategory
</commit_message>
<xml_diff>
--- a/book/management/commands/uploads/category_list1.xlsx
+++ b/book/management/commands/uploads/category_list1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -49,37 +49,46 @@
     <t xml:space="preserve">Civil Engineering</t>
   </si>
   <si>
-    <t xml:space="preserve">Medical</t>
+    <t xml:space="preserve">Computer Science and Engineering2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrical Engineering2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mechanical Engineering2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical Engineering2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civil Engineering2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neorosurgery</t>
   </si>
   <si>
     <t xml:space="preserve">Surgery</t>
   </si>
   <si>
+    <t xml:space="preserve">Ansthesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orthopedics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pediatric</t>
+  </si>
+  <si>
     <t xml:space="preserve">Medicine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gynae &amp; Obs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neorosurgery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ansthesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orthopedics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pediatric</t>
   </si>
   <si>
     <t xml:space="preserve">Cardiology</t>
@@ -210,10 +219,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -284,13 +293,16 @@
       <c r="B8" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="C8" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,7 +310,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,7 +318,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -314,7 +326,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -322,132 +334,140 @@
         <v>14</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>